<commit_message>
Criando Relacionamentos Power BI
</commit_message>
<xml_diff>
--- a/Cadastro Lojas.xlsx
+++ b/Cadastro Lojas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e775ab26b5c1cdcb/Hashtag/Aulas Power BI/Power BI Impressionador/Módulo Power Query (Novo)/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e775ab26b5c1cdcb/Hashtag/Aulas Power BI/Power BI Impressionador/Hashtag Eletro/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="11_FA66D272AA1066B08AF955C2714F872426B3E244" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D7CBCFD2-8B82-4F63-B517-1055166E96D9}"/>
+  <xr:revisionPtr revIDLastSave="32" documentId="11_FA66D272AA1066B08AF955C2714F872426B3E244" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{89F5605B-EF6D-44DD-B25C-7777D7D58C7D}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -535,7 +535,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:XFD15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>

</xml_diff>

<commit_message>
Atualizações de relacionamentos estre tabelas
</commit_message>
<xml_diff>
--- a/Cadastro Lojas.xlsx
+++ b/Cadastro Lojas.xlsx
@@ -1,34 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e775ab26b5c1cdcb/Hashtag/Aulas Power BI/Power BI Impressionador/Hashtag Eletro/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alon Pinheiro\Desktop\Power BI Impressionador\Hashtag Eletro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="11_FA66D272AA1066B08AF955C2714F872426B3E244" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{89F5605B-EF6D-44DD-B25C-7777D7D58C7D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFD05614-8C20-47DA-8483-4E7D643A6386}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Lojas" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$B$1:$C$14</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Lojas!$A$1:$C$14</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="38">
   <si>
     <t>Loja</t>
   </si>
@@ -66,6 +71,39 @@
     <t>Campinas</t>
   </si>
   <si>
+    <t>Estado</t>
+  </si>
+  <si>
+    <t>RJ</t>
+  </si>
+  <si>
+    <t>MG</t>
+  </si>
+  <si>
+    <t>BA</t>
+  </si>
+  <si>
+    <t>PR</t>
+  </si>
+  <si>
+    <t>CE</t>
+  </si>
+  <si>
+    <t>PE</t>
+  </si>
+  <si>
+    <t>RS</t>
+  </si>
+  <si>
+    <t>GO</t>
+  </si>
+  <si>
+    <t>SP</t>
+  </si>
+  <si>
+    <t>Nova Iguaço</t>
+  </si>
+  <si>
     <t>Niterói</t>
   </si>
   <si>
@@ -109,63 +147,6 @@
   </si>
   <si>
     <t>Eduardo Julianelli</t>
-  </si>
-  <si>
-    <t>Nova Iguaçu</t>
-  </si>
-  <si>
-    <t>R. Visc. de Pirajá, 136 - Ipanema, Rio de Janeiro - RJ, 22410-000</t>
-  </si>
-  <si>
-    <t>Av. Barão Homem de Melo, 1389 - Nova Granada, Belo Horizonte - MG, 30431-425</t>
-  </si>
-  <si>
-    <t>Shopping Barra - Av. Centenário, 2992 - Barra, Salvador - BA, 40155-150</t>
-  </si>
-  <si>
-    <t>R. Brasílio Itiberê, 3279 - Água Verde, Curitiba - PR, 80250-160</t>
-  </si>
-  <si>
-    <t>Av. Dom Luís, 500 - Aldeota, Fortaleza - CE, 60160-230</t>
-  </si>
-  <si>
-    <t>Rua Antônio Lumack do Monte, 203 - 1 - Boa Viagem, Recife - PE, 51020-350</t>
-  </si>
-  <si>
-    <t>Av. Borges de Medeiros, 3120 - Praia de Belas, Porto Alegre - RS, 90110-150</t>
-  </si>
-  <si>
-    <t>Av. Mal. Floriano Peixoto, 2248-2258 - Centro, Nova Iguaçu - RJ, 26210-000</t>
-  </si>
-  <si>
-    <t>R. Teodoro Sampaio, 954 - Pinheiros, São Paulo - SP, 05406-050</t>
-  </si>
-  <si>
-    <t>Rua Quinze de Novembro, 8 - Loja 301a Loja 301b - Centro, Niterói - RJ, 24020-125</t>
-  </si>
-  <si>
-    <t>Av. Goiás Norte, 3.592 - quadra 2.1 - St. Mal. Rondon, Goiânia - GO, 74063-010</t>
-  </si>
-  <si>
-    <t>R. Luíz Faccini, 212 - Centro, Guarulhos - SP, 07110-000</t>
-  </si>
-  <si>
-    <t>R. Dr. Antônio Castro Prado, 422 - Vila Rossi e Borchi, Campinas - SP, 13076-130</t>
-  </si>
-  <si>
-    <t>Endereço</t>
-  </si>
-  <si>
-    <t>RG Gerente</t>
-  </si>
-  <si>
-    <t>295498980</t>
-  </si>
-  <si>
-    <t>329056282</t>
-  </si>
-  <si>
-    <t>294681591</t>
   </si>
 </sst>
 </file>
@@ -236,7 +217,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -245,12 +226,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -533,213 +508,169 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:XFD15"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="73.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.81640625" customWidth="1"/>
+    <col min="3" max="3" width="17.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
+      <c r="C2" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="4">
-        <v>506215428</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="5">
-        <v>259267806</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="5">
-        <v>259430602</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="4">
-        <v>198870966</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="3" t="s">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="4">
-        <v>307641375</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
+      <c r="C12" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="1" t="s">
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="3" t="s">
+      <c r="C13" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="4">
-        <v>247230364</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="5">
-        <v>328196186</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" s="4">
-        <v>369595269</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="5">
-        <v>335836902</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="4">
-        <v>486616964</v>
       </c>
     </row>
   </sheetData>

</xml_diff>